<commit_message>
Add normalized list of names (camel case) and threshold ratio. Not found list must still be revised.
</commit_message>
<xml_diff>
--- a/location_names.xlsx
+++ b/location_names.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="ign" sheetId="1" r:id="rId1"/>
     <sheet name="censo2010" sheetId="2" r:id="rId2"/>
-    <sheet name="tbl_correspondence" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -80796,16 +80795,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>